<commit_message>
performance bands and tag infrastructure added
</commit_message>
<xml_diff>
--- a/app/assets/TestDataSpreadsheet.xlsx
+++ b/app/assets/TestDataSpreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="0" windowWidth="25040" windowHeight="23540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
@@ -856,7 +856,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -912,6 +912,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -921,7 +927,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="29"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="61">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -961,6 +967,12 @@
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1308,7 +1320,7 @@
   <dimension ref="A1:F100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+      <selection activeCell="F2" sqref="F2:F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1348,8 +1360,8 @@
         <v>203</v>
       </c>
       <c r="F2" t="str">
-        <f>"StudentUser.new({id:"&amp;A2&amp;" , username: """&amp;D2&amp;""", first_name: """&amp;B2&amp;""", last_name: """&amp;C2&amp;""", display_name: """&amp;B2&amp;" "&amp;C2&amp;""", email: """&amp;D2&amp;""", password: ""test""}).save"</f>
-        <v>StudentUser.new({id:1 , username: "test1@test.com", first_name: "Maria ", last_name: "Hill", display_name: "Maria  Hill", email: "test1@test.com", password: "test"}).save</v>
+        <f>"StudentUser.new({username: """&amp;D2&amp;""", first_name: """&amp;B2&amp;""", last_name: """&amp;C2&amp;""", display_name: """&amp;B2&amp;" "&amp;C2&amp;""", email: """&amp;D2&amp;""", password: ""test""}).save"</f>
+        <v>StudentUser.new({username: "test1@test.com", first_name: "Maria ", last_name: "Hill", display_name: "Maria  Hill", email: "test1@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17">
@@ -1371,8 +1383,8 @@
         <v>203</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="1">"StudentUser.new({id:"&amp;A3&amp;" , username: """&amp;D3&amp;""", first_name: """&amp;B3&amp;""", last_name: """&amp;C3&amp;""", display_name: """&amp;B3&amp;" "&amp;C3&amp;""", email: """&amp;D3&amp;""", password: ""test""}).save"</f>
-        <v>StudentUser.new({id:2 , username: "test2@test.com", first_name: "Ronald ", last_name: "Brooks", display_name: "Ronald  Brooks", email: "test2@test.com", password: "test"}).save</v>
+        <f t="shared" ref="F3:F66" si="1">"StudentUser.new({username: """&amp;D3&amp;""", first_name: """&amp;B3&amp;""", last_name: """&amp;C3&amp;""", display_name: """&amp;B3&amp;" "&amp;C3&amp;""", email: """&amp;D3&amp;""", password: ""test""}).save"</f>
+        <v>StudentUser.new({username: "test2@test.com", first_name: "Ronald ", last_name: "Brooks", display_name: "Ronald  Brooks", email: "test2@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17">
@@ -1395,7 +1407,7 @@
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:3 , username: "test3@test.com", first_name: "Lisa ", last_name: "Moore", display_name: "Lisa  Moore", email: "test3@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test3@test.com", first_name: "Lisa ", last_name: "Moore", display_name: "Lisa  Moore", email: "test3@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17">
@@ -1418,7 +1430,7 @@
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:4 , username: "test4@test.com", first_name: "Chris ", last_name: "Young", display_name: "Chris  Young", email: "test4@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test4@test.com", first_name: "Chris ", last_name: "Young", display_name: "Chris  Young", email: "test4@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17">
@@ -1441,7 +1453,7 @@
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:5 , username: "test5@test.com", first_name: "Theresa ", last_name: "Ramirez", display_name: "Theresa  Ramirez", email: "test5@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test5@test.com", first_name: "Theresa ", last_name: "Ramirez", display_name: "Theresa  Ramirez", email: "test5@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17">
@@ -1464,7 +1476,7 @@
       </c>
       <c r="F7" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:6 , username: "test6@test.com", first_name: "Anna ", last_name: "Brown", display_name: "Anna  Brown", email: "test6@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test6@test.com", first_name: "Anna ", last_name: "Brown", display_name: "Anna  Brown", email: "test6@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17">
@@ -1487,7 +1499,7 @@
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:7 , username: "test7@test.com", first_name: "Angela ", last_name: "Alexander", display_name: "Angela  Alexander", email: "test7@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test7@test.com", first_name: "Angela ", last_name: "Alexander", display_name: "Angela  Alexander", email: "test7@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17">
@@ -1510,7 +1522,7 @@
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:8 , username: "test8@test.com", first_name: "Benjamin ", last_name: "Lee", display_name: "Benjamin  Lee", email: "test8@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test8@test.com", first_name: "Benjamin ", last_name: "Lee", display_name: "Benjamin  Lee", email: "test8@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17">
@@ -1533,7 +1545,7 @@
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:9 , username: "test9@test.com", first_name: "Timothy ", last_name: "Garcia", display_name: "Timothy  Garcia", email: "test9@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test9@test.com", first_name: "Timothy ", last_name: "Garcia", display_name: "Timothy  Garcia", email: "test9@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17">
@@ -1556,7 +1568,7 @@
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:10 , username: "test10@test.com", first_name: "Sean ", last_name: "Hall", display_name: "Sean  Hall", email: "test10@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test10@test.com", first_name: "Sean ", last_name: "Hall", display_name: "Sean  Hall", email: "test10@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17">
@@ -1579,7 +1591,7 @@
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:11 , username: "test11@test.com", first_name: "Raymond ", last_name: "Williams", display_name: "Raymond  Williams", email: "test11@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test11@test.com", first_name: "Raymond ", last_name: "Williams", display_name: "Raymond  Williams", email: "test11@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17">
@@ -1602,7 +1614,7 @@
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:12 , username: "test12@test.com", first_name: "Helen ", last_name: "Diaz", display_name: "Helen  Diaz", email: "test12@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test12@test.com", first_name: "Helen ", last_name: "Diaz", display_name: "Helen  Diaz", email: "test12@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17">
@@ -1625,7 +1637,7 @@
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:13 , username: "test13@test.com", first_name: "Emily ", last_name: "Stewart", display_name: "Emily  Stewart", email: "test13@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test13@test.com", first_name: "Emily ", last_name: "Stewart", display_name: "Emily  Stewart", email: "test13@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17">
@@ -1648,7 +1660,7 @@
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:14 , username: "test14@test.com", first_name: "Alan ", last_name: "Baker", display_name: "Alan  Baker", email: "test14@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test14@test.com", first_name: "Alan ", last_name: "Baker", display_name: "Alan  Baker", email: "test14@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17">
@@ -1671,7 +1683,7 @@
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:15 , username: "test15@test.com", first_name: "Kimberly ", last_name: "Wilson", display_name: "Kimberly  Wilson", email: "test15@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test15@test.com", first_name: "Kimberly ", last_name: "Wilson", display_name: "Kimberly  Wilson", email: "test15@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17">
@@ -1694,7 +1706,7 @@
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:16 , username: "test16@test.com", first_name: "Donna ", last_name: "Bailey", display_name: "Donna  Bailey", email: "test16@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test16@test.com", first_name: "Donna ", last_name: "Bailey", display_name: "Donna  Bailey", email: "test16@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17">
@@ -1717,7 +1729,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:17 , username: "test17@test.com", first_name: "Paula ", last_name: "Rodriguez", display_name: "Paula  Rodriguez", email: "test17@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test17@test.com", first_name: "Paula ", last_name: "Rodriguez", display_name: "Paula  Rodriguez", email: "test17@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17">
@@ -1740,7 +1752,7 @@
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:18 , username: "test18@test.com", first_name: "Carlos ", last_name: "Phillips", display_name: "Carlos  Phillips", email: "test18@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test18@test.com", first_name: "Carlos ", last_name: "Phillips", display_name: "Carlos  Phillips", email: "test18@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17">
@@ -1763,7 +1775,7 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:19 , username: "test19@test.com", first_name: "James ", last_name: "Flores", display_name: "James  Flores", email: "test19@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test19@test.com", first_name: "James ", last_name: "Flores", display_name: "James  Flores", email: "test19@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17">
@@ -1786,7 +1798,7 @@
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:20 , username: "test20@test.com", first_name: "Anthony ", last_name: "Johnson", display_name: "Anthony  Johnson", email: "test20@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test20@test.com", first_name: "Anthony ", last_name: "Johnson", display_name: "Anthony  Johnson", email: "test20@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17">
@@ -1809,7 +1821,7 @@
       </c>
       <c r="F22" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:21 , username: "test21@test.com", first_name: "Clarence ", last_name: "Bryant", display_name: "Clarence  Bryant", email: "test21@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test21@test.com", first_name: "Clarence ", last_name: "Bryant", display_name: "Clarence  Bryant", email: "test21@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17">
@@ -1832,7 +1844,7 @@
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:22 , username: "test22@test.com", first_name: "Diane ", last_name: "Parker", display_name: "Diane  Parker", email: "test22@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test22@test.com", first_name: "Diane ", last_name: "Parker", display_name: "Diane  Parker", email: "test22@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17">
@@ -1855,7 +1867,7 @@
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:23 , username: "test23@test.com", first_name: "Howard ", last_name: "Miller", display_name: "Howard  Miller", email: "test23@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test23@test.com", first_name: "Howard ", last_name: "Miller", display_name: "Howard  Miller", email: "test23@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17">
@@ -1878,7 +1890,7 @@
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:24 , username: "test24@test.com", first_name: "Gary ", last_name: "Collins", display_name: "Gary  Collins", email: "test24@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test24@test.com", first_name: "Gary ", last_name: "Collins", display_name: "Gary  Collins", email: "test24@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17">
@@ -1901,7 +1913,7 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:25 , username: "test25@test.com", first_name: "Richard ", last_name: "Morgan", display_name: "Richard  Morgan", email: "test25@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test25@test.com", first_name: "Richard ", last_name: "Morgan", display_name: "Richard  Morgan", email: "test25@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17">
@@ -1924,7 +1936,7 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:26 , username: "test26@test.com", first_name: "Rachel ", last_name: "Murphy", display_name: "Rachel  Murphy", email: "test26@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test26@test.com", first_name: "Rachel ", last_name: "Murphy", display_name: "Rachel  Murphy", email: "test26@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="17">
@@ -1947,7 +1959,7 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:27 , username: "test27@test.com", first_name: "Bobby ", last_name: "Scott", display_name: "Bobby  Scott", email: "test27@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test27@test.com", first_name: "Bobby ", last_name: "Scott", display_name: "Bobby  Scott", email: "test27@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17">
@@ -1970,7 +1982,7 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:28 , username: "test28@test.com", first_name: "Harry ", last_name: "Kelly", display_name: "Harry  Kelly", email: "test28@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test28@test.com", first_name: "Harry ", last_name: "Kelly", display_name: "Harry  Kelly", email: "test28@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17">
@@ -1993,7 +2005,7 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:29 , username: "test29@test.com", first_name: "Annie ", last_name: "Anderson", display_name: "Annie  Anderson", email: "test29@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test29@test.com", first_name: "Annie ", last_name: "Anderson", display_name: "Annie  Anderson", email: "test29@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17">
@@ -2016,7 +2028,7 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:30 , username: "test30@test.com", first_name: "Joe ", last_name: "Peterson", display_name: "Joe  Peterson", email: "test30@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test30@test.com", first_name: "Joe ", last_name: "Peterson", display_name: "Joe  Peterson", email: "test30@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17">
@@ -2039,7 +2051,7 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:31 , username: "test31@test.com", first_name: "Bruce ", last_name: "Foster", display_name: "Bruce  Foster", email: "test31@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test31@test.com", first_name: "Bruce ", last_name: "Foster", display_name: "Bruce  Foster", email: "test31@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="17">
@@ -2062,7 +2074,7 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:32 , username: "test32@test.com", first_name: "Craig ", last_name: "Cooper", display_name: "Craig  Cooper", email: "test32@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test32@test.com", first_name: "Craig ", last_name: "Cooper", display_name: "Craig  Cooper", email: "test32@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17">
@@ -2085,7 +2097,7 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:33 , username: "test33@test.com", first_name: "Kathleen ", last_name: "Wood", display_name: "Kathleen  Wood", email: "test33@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test33@test.com", first_name: "Kathleen ", last_name: "Wood", display_name: "Kathleen  Wood", email: "test33@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17">
@@ -2108,7 +2120,7 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:34 , username: "test34@test.com", first_name: "Todd ", last_name: "Perez", display_name: "Todd  Perez", email: "test34@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test34@test.com", first_name: "Todd ", last_name: "Perez", display_name: "Todd  Perez", email: "test34@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="17">
@@ -2131,7 +2143,7 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:35 , username: "test35@test.com", first_name: "Jimmy ", last_name: "Gonzalez", display_name: "Jimmy  Gonzalez", email: "test35@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test35@test.com", first_name: "Jimmy ", last_name: "Gonzalez", display_name: "Jimmy  Gonzalez", email: "test35@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17">
@@ -2154,7 +2166,7 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:36 , username: "test36@test.com", first_name: "Aaron ", last_name: "Powell", display_name: "Aaron  Powell", email: "test36@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test36@test.com", first_name: "Aaron ", last_name: "Powell", display_name: "Aaron  Powell", email: "test36@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17">
@@ -2177,7 +2189,7 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:37 , username: "test37@test.com", first_name: "Stephen ", last_name: "Perry", display_name: "Stephen  Perry", email: "test37@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test37@test.com", first_name: "Stephen ", last_name: "Perry", display_name: "Stephen  Perry", email: "test37@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="17">
@@ -2200,7 +2212,7 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:38 , username: "test38@test.com", first_name: "Andrea ", last_name: "Barnes", display_name: "Andrea  Barnes", email: "test38@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test38@test.com", first_name: "Andrea ", last_name: "Barnes", display_name: "Andrea  Barnes", email: "test38@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="17">
@@ -2223,7 +2235,7 @@
       </c>
       <c r="F40" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:39 , username: "test39@test.com", first_name: "Nicole ", last_name: "Gray", display_name: "Nicole  Gray", email: "test39@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test39@test.com", first_name: "Nicole ", last_name: "Gray", display_name: "Nicole  Gray", email: "test39@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17">
@@ -2246,7 +2258,7 @@
       </c>
       <c r="F41" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:40 , username: "test40@test.com", first_name: "Linda ", last_name: "Butler", display_name: "Linda  Butler", email: "test40@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test40@test.com", first_name: "Linda ", last_name: "Butler", display_name: "Linda  Butler", email: "test40@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17">
@@ -2269,7 +2281,7 @@
       </c>
       <c r="F42" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:41 , username: "test41@test.com", first_name: "Anne ", last_name: "Clark", display_name: "Anne  Clark", email: "test41@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test41@test.com", first_name: "Anne ", last_name: "Clark", display_name: "Anne  Clark", email: "test41@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17">
@@ -2292,7 +2304,7 @@
       </c>
       <c r="F43" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:42 , username: "test42@test.com", first_name: "Douglas ", last_name: "Adams", display_name: "Douglas  Adams", email: "test42@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test42@test.com", first_name: "Douglas ", last_name: "Adams", display_name: "Douglas  Adams", email: "test42@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17">
@@ -2315,7 +2327,7 @@
       </c>
       <c r="F44" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:43 , username: "test43@test.com", first_name: "Barbara ", last_name: "Morris", display_name: "Barbara  Morris", email: "test43@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test43@test.com", first_name: "Barbara ", last_name: "Morris", display_name: "Barbara  Morris", email: "test43@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17">
@@ -2338,7 +2350,7 @@
       </c>
       <c r="F45" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:44 , username: "test44@test.com", first_name: "Kelly ", last_name: "Mitchell", display_name: "Kelly  Mitchell", email: "test44@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test44@test.com", first_name: "Kelly ", last_name: "Mitchell", display_name: "Kelly  Mitchell", email: "test44@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17">
@@ -2361,7 +2373,7 @@
       </c>
       <c r="F46" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:45 , username: "test45@test.com", first_name: "Donald ", last_name: "Griffin", display_name: "Donald  Griffin", email: "test45@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test45@test.com", first_name: "Donald ", last_name: "Griffin", display_name: "Donald  Griffin", email: "test45@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17">
@@ -2384,7 +2396,7 @@
       </c>
       <c r="F47" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:46 , username: "test46@test.com", first_name: "Susan ", last_name: "Harris", display_name: "Susan  Harris", email: "test46@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test46@test.com", first_name: "Susan ", last_name: "Harris", display_name: "Susan  Harris", email: "test46@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17">
@@ -2407,7 +2419,7 @@
       </c>
       <c r="F48" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:47 , username: "test47@test.com", first_name: "Joseph ", last_name: "Thompson", display_name: "Joseph  Thompson", email: "test47@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test47@test.com", first_name: "Joseph ", last_name: "Thompson", display_name: "Joseph  Thompson", email: "test47@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17">
@@ -2430,7 +2442,7 @@
       </c>
       <c r="F49" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:48 , username: "test48@test.com", first_name: "Margaret ", last_name: "Evans", display_name: "Margaret  Evans", email: "test48@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test48@test.com", first_name: "Margaret ", last_name: "Evans", display_name: "Margaret  Evans", email: "test48@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17">
@@ -2453,7 +2465,7 @@
       </c>
       <c r="F50" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:49 , username: "test49@test.com", first_name: "Thomas ", last_name: "Reed", display_name: "Thomas  Reed", email: "test49@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test49@test.com", first_name: "Thomas ", last_name: "Reed", display_name: "Thomas  Reed", email: "test49@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17">
@@ -2476,7 +2488,7 @@
       </c>
       <c r="F51" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:50 , username: "test50@test.com", first_name: "Judy ", last_name: "Wright", display_name: "Judy  Wright", email: "test50@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test50@test.com", first_name: "Judy ", last_name: "Wright", display_name: "Judy  Wright", email: "test50@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17">
@@ -2499,7 +2511,7 @@
       </c>
       <c r="F52" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:51 , username: "test51@test.com", first_name: "George ", last_name: "Henderson", display_name: "George  Henderson", email: "test51@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test51@test.com", first_name: "George ", last_name: "Henderson", display_name: "George  Henderson", email: "test51@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17">
@@ -2522,7 +2534,7 @@
       </c>
       <c r="F53" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:52 , username: "test52@test.com", first_name: "Fred ", last_name: "Lewis", display_name: "Fred  Lewis", email: "test52@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test52@test.com", first_name: "Fred ", last_name: "Lewis", display_name: "Fred  Lewis", email: "test52@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17">
@@ -2545,7 +2557,7 @@
       </c>
       <c r="F54" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:53 , username: "test53@test.com", first_name: "Jessica ", last_name: "Ward", display_name: "Jessica  Ward", email: "test53@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test53@test.com", first_name: "Jessica ", last_name: "Ward", display_name: "Jessica  Ward", email: "test53@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17">
@@ -2568,7 +2580,7 @@
       </c>
       <c r="F55" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:54 , username: "test54@test.com", first_name: "Victor ", last_name: "Cook", display_name: "Victor  Cook", email: "test54@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test54@test.com", first_name: "Victor ", last_name: "Cook", display_name: "Victor  Cook", email: "test54@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17">
@@ -2591,7 +2603,7 @@
       </c>
       <c r="F56" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:55 , username: "test55@test.com", first_name: "Judith ", last_name: "Campbell", display_name: "Judith  Campbell", email: "test55@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test55@test.com", first_name: "Judith ", last_name: "Campbell", display_name: "Judith  Campbell", email: "test55@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17">
@@ -2614,7 +2626,7 @@
       </c>
       <c r="F57" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:56 , username: "test56@test.com", first_name: "Rebecca ", last_name: "Watson", display_name: "Rebecca  Watson", email: "test56@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test56@test.com", first_name: "Rebecca ", last_name: "Watson", display_name: "Rebecca  Watson", email: "test56@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17">
@@ -2637,7 +2649,7 @@
       </c>
       <c r="F58" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:57 , username: "test57@test.com", first_name: "Frank ", last_name: "Nelson", display_name: "Frank  Nelson", email: "test57@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test57@test.com", first_name: "Frank ", last_name: "Nelson", display_name: "Frank  Nelson", email: "test57@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17">
@@ -2660,7 +2672,7 @@
       </c>
       <c r="F59" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:58 , username: "test58@test.com", first_name: "Marie ", last_name: "Hernandez", display_name: "Marie  Hernandez", email: "test58@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test58@test.com", first_name: "Marie ", last_name: "Hernandez", display_name: "Marie  Hernandez", email: "test58@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17">
@@ -2683,7 +2695,7 @@
       </c>
       <c r="F60" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:59 , username: "test59@test.com", first_name: "Louise ", last_name: "Roberts", display_name: "Louise  Roberts", email: "test59@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test59@test.com", first_name: "Louise ", last_name: "Roberts", display_name: "Louise  Roberts", email: "test59@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17">
@@ -2706,7 +2718,7 @@
       </c>
       <c r="F61" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:60 , username: "test60@test.com", first_name: "Lillian ", last_name: "Price", display_name: "Lillian  Price", email: "test60@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test60@test.com", first_name: "Lillian ", last_name: "Price", display_name: "Lillian  Price", email: "test60@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17">
@@ -2729,7 +2741,7 @@
       </c>
       <c r="F62" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:61 , username: "test61@test.com", first_name: "Carl ", last_name: "Richardson", display_name: "Carl  Richardson", email: "test61@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test61@test.com", first_name: "Carl ", last_name: "Richardson", display_name: "Carl  Richardson", email: "test61@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17">
@@ -2752,7 +2764,7 @@
       </c>
       <c r="F63" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:62 , username: "test62@test.com", first_name: "Bonnie ", last_name: "Jackson", display_name: "Bonnie  Jackson", email: "test62@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test62@test.com", first_name: "Bonnie ", last_name: "Jackson", display_name: "Bonnie  Jackson", email: "test62@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17">
@@ -2775,7 +2787,7 @@
       </c>
       <c r="F64" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:63 , username: "test63@test.com", first_name: "Deborah ", last_name: "Carter", display_name: "Deborah  Carter", email: "test63@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test63@test.com", first_name: "Deborah ", last_name: "Carter", display_name: "Deborah  Carter", email: "test63@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="17">
@@ -2798,7 +2810,7 @@
       </c>
       <c r="F65" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:64 , username: "test64@test.com", first_name: "Steven ", last_name: "Howard", display_name: "Steven  Howard", email: "test64@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test64@test.com", first_name: "Steven ", last_name: "Howard", display_name: "Steven  Howard", email: "test64@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="17">
@@ -2821,7 +2833,7 @@
       </c>
       <c r="F66" t="str">
         <f t="shared" si="1"/>
-        <v>StudentUser.new({id:65 , username: "test65@test.com", first_name: "Heather ", last_name: "Smith", display_name: "Heather  Smith", email: "test65@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test65@test.com", first_name: "Heather ", last_name: "Smith", display_name: "Heather  Smith", email: "test65@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="17">
@@ -2843,8 +2855,8 @@
         <v>203</v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F100" si="4">"StudentUser.new({id:"&amp;A67&amp;" , username: """&amp;D67&amp;""", first_name: """&amp;B67&amp;""", last_name: """&amp;C67&amp;""", display_name: """&amp;B67&amp;" "&amp;C67&amp;""", email: """&amp;D67&amp;""", password: ""test""}).save"</f>
-        <v>StudentUser.new({id:66 , username: "test66@test.com", first_name: "Mark ", last_name: "Gonzales", display_name: "Mark  Gonzales", email: "test66@test.com", password: "test"}).save</v>
+        <f t="shared" ref="F67:F100" si="4">"StudentUser.new({username: """&amp;D67&amp;""", first_name: """&amp;B67&amp;""", last_name: """&amp;C67&amp;""", display_name: """&amp;B67&amp;" "&amp;C67&amp;""", email: """&amp;D67&amp;""", password: ""test""}).save"</f>
+        <v>StudentUser.new({username: "test66@test.com", first_name: "Mark ", last_name: "Gonzales", display_name: "Mark  Gonzales", email: "test66@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="17">
@@ -2867,7 +2879,7 @@
       </c>
       <c r="F68" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:67 , username: "test67@test.com", first_name: "Jane ", last_name: "Robinson", display_name: "Jane  Robinson", email: "test67@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test67@test.com", first_name: "Jane ", last_name: "Robinson", display_name: "Jane  Robinson", email: "test67@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="17">
@@ -2890,7 +2902,7 @@
       </c>
       <c r="F69" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:68 , username: "test68@test.com", first_name: "Brenda ", last_name: "Davis", display_name: "Brenda  Davis", email: "test68@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test68@test.com", first_name: "Brenda ", last_name: "Davis", display_name: "Brenda  Davis", email: "test68@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="17">
@@ -2913,7 +2925,7 @@
       </c>
       <c r="F70" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:69 , username: "test69@test.com", first_name: "Jack ", last_name: "Coleman", display_name: "Jack  Coleman", email: "test69@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test69@test.com", first_name: "Jack ", last_name: "Coleman", display_name: "Jack  Coleman", email: "test69@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="17">
@@ -2936,7 +2948,7 @@
       </c>
       <c r="F71" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:70 , username: "test70@test.com", first_name: "Phillip ", last_name: "Taylor", display_name: "Phillip  Taylor", email: "test70@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test70@test.com", first_name: "Phillip ", last_name: "Taylor", display_name: "Phillip  Taylor", email: "test70@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="17">
@@ -2959,7 +2971,7 @@
       </c>
       <c r="F72" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:71 , username: "test71@test.com", first_name: "Lois ", last_name: "Green", display_name: "Lois  Green", email: "test71@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test71@test.com", first_name: "Lois ", last_name: "Green", display_name: "Lois  Green", email: "test71@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="17">
@@ -2982,7 +2994,7 @@
       </c>
       <c r="F73" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:72 , username: "test72@test.com", first_name: "Albert ", last_name: "Sanders", display_name: "Albert  Sanders", email: "test72@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test72@test.com", first_name: "Albert ", last_name: "Sanders", display_name: "Albert  Sanders", email: "test72@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="17">
@@ -3005,7 +3017,7 @@
       </c>
       <c r="F74" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:73 , username: "test73@test.com", first_name: "Stephanie ", last_name: "Simmons", display_name: "Stephanie  Simmons", email: "test73@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test73@test.com", first_name: "Stephanie ", last_name: "Simmons", display_name: "Stephanie  Simmons", email: "test73@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="17">
@@ -3028,7 +3040,7 @@
       </c>
       <c r="F75" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:74 , username: "test74@test.com", first_name: "Randy ", last_name: "Russell", display_name: "Randy  Russell", email: "test74@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test74@test.com", first_name: "Randy ", last_name: "Russell", display_name: "Randy  Russell", email: "test74@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="17">
@@ -3051,7 +3063,7 @@
       </c>
       <c r="F76" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:75 , username: "test75@test.com", first_name: "Charles ", last_name: "Thomas", display_name: "Charles  Thomas", email: "test75@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test75@test.com", first_name: "Charles ", last_name: "Thomas", display_name: "Charles  Thomas", email: "test75@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="17">
@@ -3074,7 +3086,7 @@
       </c>
       <c r="F77" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:76 , username: "test76@test.com", first_name: "John ", last_name: "Hughes", display_name: "John  Hughes", email: "test76@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test76@test.com", first_name: "John ", last_name: "Hughes", display_name: "John  Hughes", email: "test76@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="17">
@@ -3097,7 +3109,7 @@
       </c>
       <c r="F78" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:77 , username: "test77@test.com", first_name: "Eric ", last_name: "Edwards", display_name: "Eric  Edwards", email: "test77@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test77@test.com", first_name: "Eric ", last_name: "Edwards", display_name: "Eric  Edwards", email: "test77@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="17">
@@ -3120,7 +3132,7 @@
       </c>
       <c r="F79" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:78 , username: "test78@test.com", first_name: "Jean ", last_name: "Sanchez", display_name: "Jean  Sanchez", email: "test78@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test78@test.com", first_name: "Jean ", last_name: "Sanchez", display_name: "Jean  Sanchez", email: "test78@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17">
@@ -3143,7 +3155,7 @@
       </c>
       <c r="F80" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:79 , username: "test79@test.com", first_name: "Nancy ", last_name: "Rivera", display_name: "Nancy  Rivera", email: "test79@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test79@test.com", first_name: "Nancy ", last_name: "Rivera", display_name: "Nancy  Rivera", email: "test79@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="17">
@@ -3166,7 +3178,7 @@
       </c>
       <c r="F81" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:80 , username: "test80@test.com", first_name: "Keith ", last_name: "Martin", display_name: "Keith  Martin", email: "test80@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test80@test.com", first_name: "Keith ", last_name: "Martin", display_name: "Keith  Martin", email: "test80@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="17">
@@ -3189,7 +3201,7 @@
       </c>
       <c r="F82" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:81 , username: "test81@test.com", first_name: "Robert ", last_name: "Turner", display_name: "Robert  Turner", email: "test81@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test81@test.com", first_name: "Robert ", last_name: "Turner", display_name: "Robert  Turner", email: "test81@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="17">
@@ -3212,7 +3224,7 @@
       </c>
       <c r="F83" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:82 , username: "test82@test.com", first_name: "Ralph ", last_name: "Torres", display_name: "Ralph  Torres", email: "test82@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test82@test.com", first_name: "Ralph ", last_name: "Torres", display_name: "Ralph  Torres", email: "test82@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="17">
@@ -3235,7 +3247,7 @@
       </c>
       <c r="F84" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:83 , username: "test83@test.com", first_name: "Arthur ", last_name: "Washington", display_name: "Arthur  Washington", email: "test83@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test83@test.com", first_name: "Arthur ", last_name: "Washington", display_name: "Arthur  Washington", email: "test83@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="17">
@@ -3258,7 +3270,7 @@
       </c>
       <c r="F85" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:84 , username: "test84@test.com", first_name: "Cheryl ", last_name: "Long", display_name: "Cheryl  Long", email: "test84@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test84@test.com", first_name: "Cheryl ", last_name: "Long", display_name: "Cheryl  Long", email: "test84@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="17">
@@ -3281,7 +3293,7 @@
       </c>
       <c r="F86" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:85 , username: "test85@test.com", first_name: "Lawrence ", last_name: "Patterson", display_name: "Lawrence  Patterson", email: "test85@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test85@test.com", first_name: "Lawrence ", last_name: "Patterson", display_name: "Lawrence  Patterson", email: "test85@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="17">
@@ -3304,7 +3316,7 @@
       </c>
       <c r="F87" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:86 , username: "test86@test.com", first_name: "Roger ", last_name: "Bennett", display_name: "Roger  Bennett", email: "test86@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test86@test.com", first_name: "Roger ", last_name: "Bennett", display_name: "Roger  Bennett", email: "test86@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="17">
@@ -3327,7 +3339,7 @@
       </c>
       <c r="F88" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:87 , username: "test87@test.com", first_name: "Norma ", last_name: "Bell", display_name: "Norma  Bell", email: "test87@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test87@test.com", first_name: "Norma ", last_name: "Bell", display_name: "Norma  Bell", email: "test87@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="17">
@@ -3350,7 +3362,7 @@
       </c>
       <c r="F89" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:88 , username: "test88@test.com", first_name: "Kathryn ", last_name: "King", display_name: "Kathryn  King", email: "test88@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test88@test.com", first_name: "Kathryn ", last_name: "King", display_name: "Kathryn  King", email: "test88@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="17">
@@ -3373,7 +3385,7 @@
       </c>
       <c r="F90" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:89 , username: "test89@test.com", first_name: "Teresa ", last_name: "Allen", display_name: "Teresa  Allen", email: "test89@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test89@test.com", first_name: "Teresa ", last_name: "Allen", display_name: "Teresa  Allen", email: "test89@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="17">
@@ -3396,7 +3408,7 @@
       </c>
       <c r="F91" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:90 , username: "test90@test.com", first_name: "Ruby ", last_name: "White", display_name: "Ruby  White", email: "test90@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test90@test.com", first_name: "Ruby ", last_name: "White", display_name: "Ruby  White", email: "test90@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="17">
@@ -3419,7 +3431,7 @@
       </c>
       <c r="F92" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:91 , username: "test91@test.com", first_name: "Joyce ", last_name: "Walker", display_name: "Joyce  Walker", email: "test91@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test91@test.com", first_name: "Joyce ", last_name: "Walker", display_name: "Joyce  Walker", email: "test91@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="17">
@@ -3442,7 +3454,7 @@
       </c>
       <c r="F93" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:92 , username: "test92@test.com", first_name: "Larry ", last_name: "Jones", display_name: "Larry  Jones", email: "test92@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test92@test.com", first_name: "Larry ", last_name: "Jones", display_name: "Larry  Jones", email: "test92@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="17">
@@ -3465,7 +3477,7 @@
       </c>
       <c r="F94" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:93 , username: "test93@test.com", first_name: "Sarah ", last_name: "Cox", display_name: "Sarah  Cox", email: "test93@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test93@test.com", first_name: "Sarah ", last_name: "Cox", display_name: "Sarah  Cox", email: "test93@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="17">
@@ -3488,7 +3500,7 @@
       </c>
       <c r="F95" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:94 , username: "test94@test.com", first_name: "Henry ", last_name: "Jenkins", display_name: "Henry  Jenkins", email: "test94@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test94@test.com", first_name: "Henry ", last_name: "Jenkins", display_name: "Henry  Jenkins", email: "test94@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="17">
@@ -3511,7 +3523,7 @@
       </c>
       <c r="F96" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:95 , username: "test95@test.com", first_name: "Julie ", last_name: "Lopez", display_name: "Julie  Lopez", email: "test95@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test95@test.com", first_name: "Julie ", last_name: "Lopez", display_name: "Julie  Lopez", email: "test95@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="17">
@@ -3534,7 +3546,7 @@
       </c>
       <c r="F97" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:96 , username: "test96@test.com", first_name: "Virginia ", last_name: "James", display_name: "Virginia  James", email: "test96@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test96@test.com", first_name: "Virginia ", last_name: "James", display_name: "Virginia  James", email: "test96@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="17">
@@ -3557,7 +3569,7 @@
       </c>
       <c r="F98" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:97 , username: "test97@test.com", first_name: "Lori ", last_name: "Ross", display_name: "Lori  Ross", email: "test97@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test97@test.com", first_name: "Lori ", last_name: "Ross", display_name: "Lori  Ross", email: "test97@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="17">
@@ -3580,7 +3592,7 @@
       </c>
       <c r="F99" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:98 , username: "test98@test.com", first_name: "Joan ", last_name: "Rogers", display_name: "Joan  Rogers", email: "test98@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test98@test.com", first_name: "Joan ", last_name: "Rogers", display_name: "Joan  Rogers", email: "test98@test.com", password: "test"}).save</v>
       </c>
     </row>
     <row r="100" spans="1:6" ht="17">
@@ -3603,7 +3615,7 @@
       </c>
       <c r="F100" t="str">
         <f t="shared" si="4"/>
-        <v>StudentUser.new({id:99 , username: "test99@test.com", first_name: "Sara ", last_name: "Martinez", display_name: "Sara  Martinez", email: "test99@test.com", password: "test"}).save</v>
+        <v>StudentUser.new({username: "test99@test.com", first_name: "Sara ", last_name: "Martinez", display_name: "Sara  Martinez", email: "test99@test.com", password: "test"}).save</v>
       </c>
     </row>
   </sheetData>
@@ -3621,8 +3633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3641,8 +3653,8 @@
         <v>231</v>
       </c>
       <c r="E1" t="str">
-        <f>"Activity.new({id: "&amp;A1&amp;", name:"""&amp;B1&amp;""", description: """&amp;C1&amp;""", instructions: """&amp;D1&amp;""", teacher_user_id: 100, activity_type: ""scored""}).save"</f>
-        <v>Activity.new({id: 1, name:"Multiplication", description: "ThatQuiz", instructions: "90%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <f>"Activity.new({name:"""&amp;B1&amp;""", description: """&amp;C1&amp;""", instructions: """&amp;D1&amp;""", teacher_user_id: 1, activity_type: ""scored""}).save"</f>
+        <v>Activity.new({name:"Multiplication", description: "ThatQuiz", instructions: "90%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -3684,8 +3696,8 @@
         <v>232</v>
       </c>
       <c r="E2" t="str">
-        <f t="shared" ref="E2:E24" si="0">"Activity.new({id: "&amp;A2&amp;", name:"""&amp;B2&amp;""", description: """&amp;C2&amp;""", instructions: """&amp;D2&amp;""", teacher_user_id: 100, activity_type: ""scored""}).save"</f>
-        <v>Activity.new({id: 2, name:"Division", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <f t="shared" ref="E2:E24" si="0">"Activity.new({name:"""&amp;B2&amp;""", description: """&amp;C2&amp;""", instructions: """&amp;D2&amp;""", teacher_user_id: 1, activity_type: ""scored""}).save"</f>
+        <v>Activity.new({name:"Division", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -3704,7 +3716,7 @@
       </c>
       <c r="E3" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 3, name:"Long Division1", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Long Division1", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
@@ -3725,7 +3737,7 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 4, name:"Long Division2", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Long Division2", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -3746,7 +3758,7 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 5, name:"Long Division3", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Long Division3", description: "ThatQuiz", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
@@ -3767,7 +3779,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 6, name:"Multiplication without carrying", description: "Khan", instructions: "5 in a row", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Multiplication without carrying", description: "Khan", instructions: "5 in a row", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -3788,7 +3800,7 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 7, name:"Multiplication with carrying", description: "Khan", instructions: "5 in a row", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Multiplication with carrying", description: "Khan", instructions: "5 in a row", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
@@ -3809,7 +3821,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 8, name:"Multiplying 2 digits by 2 digits", description: "Khan", instructions: "5 in a row", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Multiplying 2 digits by 2 digits", description: "Khan", instructions: "5 in a row", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -3830,7 +3842,7 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 9, name:"Multi-digit division without remainders", description: "Khan", instructions: "5 in a row", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Multi-digit division without remainders", description: "Khan", instructions: "5 in a row", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
@@ -3851,7 +3863,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 10, name:"Division with remainders", description: "Khan", instructions: "5 in a row", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Division with remainders", description: "Khan", instructions: "5 in a row", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
@@ -3872,7 +3884,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 11, name:"Multiplication and division word problems", description: "Khan", instructions: "5 in a row", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"Multiplication and division word problems", description: "Khan", instructions: "5 in a row", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -3893,7 +3905,7 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 12, name:"GCF", description: "Khan", instructions: "5 in a row", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"GCF", description: "Khan", instructions: "5 in a row", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -3914,7 +3926,7 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 13, name:"L3: Fluently Solve Multiplication Problems", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L3: Fluently Solve Multiplication Problems", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -3935,7 +3947,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 14, name:"L3: Fluently Solve Division Problems", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L3: Fluently Solve Division Problems", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -3956,7 +3968,7 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 15, name:"L3: Solving Multiplication and Division Verbally", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L3: Solving Multiplication and Division Verbally", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -3977,7 +3989,7 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 16, name:"L4: Multiplication and Division Strategies", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L4: Multiplication and Division Strategies", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -3998,7 +4010,7 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 17, name:"L4: Factors", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L4: Factors", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -4019,7 +4031,7 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 18, name:"L4: Relating Multiplication and Division", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L4: Relating Multiplication and Division", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -4040,7 +4052,7 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 19, name:"L5: Multiplication with Multi-Digit Whole Numbers", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L5: Multiplication with Multi-Digit Whole Numbers", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -4061,7 +4073,7 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 20, name:"L5: Dividing Whole Numbers", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L5: Dividing Whole Numbers", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -4082,7 +4094,7 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 21, name:"L5: Complete Equivalent Fractions", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L5: Complete Equivalent Fractions", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -4103,7 +4115,7 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 22, name:"L5: Finding Equivalent Fractions and Fractions in Simplest Form", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L5: Finding Equivalent Fractions and Fractions in Simplest Form", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -4124,7 +4136,7 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 23, name:"L6: Identifying the Least Common Multiple", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L6: Identifying the Least Common Multiple", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -4145,7 +4157,7 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
-        <v>Activity.new({id: 24, name:"L6: Identifying the Greatest Common Factor", description: "TenMarks", instructions: "80%+", teacher_user_id: 100, activity_type: "scored"}).save</v>
+        <v>Activity.new({name:"L6: Identifying the Greatest Common Factor", description: "TenMarks", instructions: "80%+", teacher_user_id: 1, activity_type: "scored"}).save</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -4174,7 +4186,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="A1:E3"/>
+      <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4213,8 +4225,8 @@
         <v>203</v>
       </c>
       <c r="F2" t="str">
-        <f>"TeacherUser.new({id:"&amp;A2&amp;" , username: """&amp;D2&amp;""", first_name: """&amp;B2&amp;""", last_name: """&amp;C2&amp;""", display_name: """&amp;B2&amp;" "&amp;C2&amp;""", email: """&amp;D2&amp;""", password: ""test""}).save"</f>
-        <v>TeacherUser.new({id:100 , username: "dli@sjusd.org", first_name: "Dennis", last_name: "Li", display_name: "Dennis Li", email: "dli@sjusd.org", password: "test"}).save</v>
+        <f>"TeacherUser.new({username: """&amp;D2&amp;""", first_name: """&amp;B2&amp;""", last_name: """&amp;C2&amp;""", display_name: """&amp;B2&amp;" "&amp;C2&amp;""", email: """&amp;D2&amp;""", password: ""test""}).save"</f>
+        <v>TeacherUser.new({username: "dli@sjusd.org", first_name: "Dennis", last_name: "Li", display_name: "Dennis Li", email: "dli@sjusd.org", password: "test"}).save</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -4234,8 +4246,8 @@
         <v>203</v>
       </c>
       <c r="F3" t="str">
-        <f>"TeacherUser.new({id:"&amp;A3&amp;" , username: """&amp;D3&amp;""", first_name: """&amp;B3&amp;""", last_name: """&amp;C3&amp;""", display_name: """&amp;B3&amp;" "&amp;C3&amp;""", email: """&amp;D3&amp;""", password: ""test""}).save"</f>
-        <v>TeacherUser.new({id:101 , username: "rgupta@sjusd.org", first_name: "Rupa", last_name: "Gupta", display_name: "Rupa Gupta", email: "rgupta@sjusd.org", password: "test"}).save</v>
+        <f>"TeacherUser.new({username: """&amp;D3&amp;""", first_name: """&amp;B3&amp;""", last_name: """&amp;C3&amp;""", display_name: """&amp;B3&amp;" "&amp;C3&amp;""", email: """&amp;D3&amp;""", password: ""test""}).save"</f>
+        <v>TeacherUser.new({username: "rgupta@sjusd.org", first_name: "Rupa", last_name: "Gupta", display_name: "Rupa Gupta", email: "rgupta@sjusd.org", password: "test"}).save</v>
       </c>
     </row>
   </sheetData>
@@ -4361,7 +4373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C49"/>
     </sheetView>
   </sheetViews>
@@ -5034,7 +5046,7 @@
     <row r="2" spans="1:5">
       <c r="A2">
         <f ca="1">CEILING(RAND()*99,1)</f>
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <f ca="1">CEILING(RAND()*3,1)</f>
@@ -5053,12 +5065,12 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <f t="shared" ref="A3:C66" ca="1" si="0">CEILING(RAND()*99,1)</f>
-        <v>48</v>
+        <f t="shared" ref="A3:A66" ca="1" si="0">CEILING(RAND()*99,1)</f>
+        <v>55</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:D66" ca="1" si="1">CEILING(RAND()*3,1)</f>
-        <v>2</v>
+        <f t="shared" ref="B3:B66" ca="1" si="1">CEILING(RAND()*3,1)</f>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>87</v>
@@ -5074,7 +5086,7 @@
     <row r="4" spans="1:5">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
@@ -5094,11 +5106,11 @@
     <row r="5" spans="1:5">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>95</v>
@@ -5114,11 +5126,11 @@
     <row r="6" spans="1:5">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>32</v>
@@ -5134,11 +5146,11 @@
     <row r="7" spans="1:5">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>19</v>
@@ -5154,11 +5166,11 @@
     <row r="8" spans="1:5">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
         <v>37</v>
@@ -5174,11 +5186,11 @@
     <row r="9" spans="1:5">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>61</v>
@@ -5194,11 +5206,11 @@
     <row r="10" spans="1:5">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10">
         <v>98</v>
@@ -5214,7 +5226,7 @@
     <row r="11" spans="1:5">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
@@ -5234,11 +5246,11 @@
     <row r="12" spans="1:5">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>51</v>
@@ -5254,11 +5266,11 @@
     <row r="13" spans="1:5">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>49</v>
@@ -5274,11 +5286,11 @@
     <row r="14" spans="1:5">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>59</v>
@@ -5294,11 +5306,11 @@
     <row r="15" spans="1:5">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>17</v>
@@ -5314,11 +5326,11 @@
     <row r="16" spans="1:5">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16">
         <v>86</v>
@@ -5334,11 +5346,11 @@
     <row r="17" spans="1:5">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>65</v>
@@ -5354,11 +5366,11 @@
     <row r="18" spans="1:5">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C18">
         <v>54</v>
@@ -5374,11 +5386,11 @@
     <row r="19" spans="1:5">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>11</v>
@@ -5394,11 +5406,11 @@
     <row r="20" spans="1:5">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>76</v>
@@ -5414,7 +5426,7 @@
     <row r="21" spans="1:5">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
@@ -5434,11 +5446,11 @@
     <row r="22" spans="1:5">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <v>34</v>
@@ -5454,7 +5466,7 @@
     <row r="23" spans="1:5">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
@@ -5474,11 +5486,11 @@
     <row r="24" spans="1:5">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <v>66</v>
@@ -5494,11 +5506,11 @@
     <row r="25" spans="1:5">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>49</v>
@@ -5514,11 +5526,11 @@
     <row r="26" spans="1:5">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C26">
         <v>65</v>
@@ -5534,7 +5546,7 @@
     <row r="27" spans="1:5">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
@@ -5554,7 +5566,7 @@
     <row r="28" spans="1:5">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>84</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
@@ -5574,7 +5586,7 @@
     <row r="29" spans="1:5">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B29">
         <f t="shared" ca="1" si="1"/>
@@ -5594,11 +5606,11 @@
     <row r="30" spans="1:5">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B30">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>81</v>
@@ -5614,11 +5626,11 @@
     <row r="31" spans="1:5">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B31">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>99</v>
@@ -5634,11 +5646,11 @@
     <row r="32" spans="1:5">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="B32">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C32">
         <v>66</v>
@@ -5654,7 +5666,7 @@
     <row r="33" spans="1:5">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B33">
         <f t="shared" ca="1" si="1"/>
@@ -5674,11 +5686,11 @@
     <row r="34" spans="1:5">
       <c r="A34">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34">
         <v>92</v>
@@ -5694,7 +5706,7 @@
     <row r="35" spans="1:5">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="B35">
         <f t="shared" ca="1" si="1"/>
@@ -5714,11 +5726,11 @@
     <row r="36" spans="1:5">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B36">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>89</v>
@@ -5734,7 +5746,7 @@
     <row r="37" spans="1:5">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <f t="shared" ca="1" si="1"/>
@@ -5754,11 +5766,11 @@
     <row r="38" spans="1:5">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="B38">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>22</v>
@@ -5774,11 +5786,11 @@
     <row r="39" spans="1:5">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B39">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>68</v>
@@ -5794,11 +5806,11 @@
     <row r="40" spans="1:5">
       <c r="A40">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="B40">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>57</v>
@@ -5814,7 +5826,7 @@
     <row r="41" spans="1:5">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="B41">
         <f t="shared" ca="1" si="1"/>
@@ -5834,11 +5846,11 @@
     <row r="42" spans="1:5">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B42">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -5854,7 +5866,7 @@
     <row r="43" spans="1:5">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="B43">
         <f t="shared" ca="1" si="1"/>
@@ -5874,7 +5886,7 @@
     <row r="44" spans="1:5">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="B44">
         <f t="shared" ca="1" si="1"/>
@@ -5894,7 +5906,7 @@
     <row r="45" spans="1:5">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B45">
         <f t="shared" ca="1" si="1"/>
@@ -5914,7 +5926,7 @@
     <row r="46" spans="1:5">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="B46">
         <f t="shared" ca="1" si="1"/>
@@ -5934,11 +5946,11 @@
     <row r="47" spans="1:5">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B47">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C47">
         <v>32</v>
@@ -5954,11 +5966,11 @@
     <row r="48" spans="1:5">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="B48">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C48">
         <v>21</v>
@@ -5974,7 +5986,7 @@
     <row r="49" spans="1:5">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="B49">
         <f t="shared" ca="1" si="1"/>
@@ -5994,11 +6006,11 @@
     <row r="50" spans="1:5">
       <c r="A50">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B50">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C50">
         <v>18</v>
@@ -6014,11 +6026,11 @@
     <row r="51" spans="1:5">
       <c r="A51">
         <f t="shared" ca="1" si="0"/>
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B51">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C51">
         <v>77</v>
@@ -6034,11 +6046,11 @@
     <row r="52" spans="1:5">
       <c r="A52">
         <f t="shared" ca="1" si="0"/>
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="B52">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52">
         <v>39</v>
@@ -6054,11 +6066,11 @@
     <row r="53" spans="1:5">
       <c r="A53">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B53">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C53">
         <v>84</v>
@@ -6074,11 +6086,11 @@
     <row r="54" spans="1:5">
       <c r="A54">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B54">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C54">
         <v>69</v>
@@ -6094,11 +6106,11 @@
     <row r="55" spans="1:5">
       <c r="A55">
         <f t="shared" ca="1" si="0"/>
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="B55">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C55">
         <v>60</v>
@@ -6114,11 +6126,11 @@
     <row r="56" spans="1:5">
       <c r="A56">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="B56">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C56">
         <v>72</v>
@@ -6134,7 +6146,7 @@
     <row r="57" spans="1:5">
       <c r="A57">
         <f t="shared" ca="1" si="0"/>
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B57">
         <f t="shared" ca="1" si="1"/>
@@ -6154,11 +6166,11 @@
     <row r="58" spans="1:5">
       <c r="A58">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>81</v>
       </c>
       <c r="B58">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C58">
         <v>77</v>
@@ -6174,7 +6186,7 @@
     <row r="59" spans="1:5">
       <c r="A59">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B59">
         <f t="shared" ca="1" si="1"/>
@@ -6194,11 +6206,11 @@
     <row r="60" spans="1:5">
       <c r="A60">
         <f t="shared" ca="1" si="0"/>
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="B60">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C60">
         <v>25</v>
@@ -6214,11 +6226,11 @@
     <row r="61" spans="1:5">
       <c r="A61">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B61">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>51</v>
@@ -6234,11 +6246,11 @@
     <row r="62" spans="1:5">
       <c r="A62">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="B62">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C62">
         <v>19</v>
@@ -6254,11 +6266,11 @@
     <row r="63" spans="1:5">
       <c r="A63">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="B63">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>35</v>
@@ -6274,11 +6286,11 @@
     <row r="64" spans="1:5">
       <c r="A64">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B64">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>21</v>
@@ -6294,11 +6306,11 @@
     <row r="65" spans="1:5">
       <c r="A65">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65">
         <v>36</v>
@@ -6314,7 +6326,7 @@
     <row r="66" spans="1:5">
       <c r="A66">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B66">
         <f t="shared" ca="1" si="1"/>
@@ -6333,12 +6345,12 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67">
-        <f t="shared" ref="A67:C130" ca="1" si="3">CEILING(RAND()*99,1)</f>
-        <v>3</v>
+        <f t="shared" ref="A67:A130" ca="1" si="3">CEILING(RAND()*99,1)</f>
+        <v>10</v>
       </c>
       <c r="B67">
-        <f t="shared" ref="B67:D130" ca="1" si="4">CEILING(RAND()*3,1)</f>
-        <v>1</v>
+        <f t="shared" ref="B67:B130" ca="1" si="4">CEILING(RAND()*3,1)</f>
+        <v>2</v>
       </c>
       <c r="C67">
         <v>85</v>
@@ -6354,11 +6366,11 @@
     <row r="68" spans="1:5">
       <c r="A68">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B68">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C68">
         <v>52</v>
@@ -6374,11 +6386,11 @@
     <row r="69" spans="1:5">
       <c r="A69">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="B69">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>32</v>
@@ -6394,11 +6406,11 @@
     <row r="70" spans="1:5">
       <c r="A70">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B70">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C70">
         <v>19</v>
@@ -6414,11 +6426,11 @@
     <row r="71" spans="1:5">
       <c r="A71">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B71">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C71">
         <v>60</v>
@@ -6434,11 +6446,11 @@
     <row r="72" spans="1:5">
       <c r="A72">
         <f t="shared" ca="1" si="3"/>
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B72">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72">
         <v>95</v>
@@ -6454,11 +6466,11 @@
     <row r="73" spans="1:5">
       <c r="A73">
         <f t="shared" ca="1" si="3"/>
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B73">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C73">
         <v>86</v>
@@ -6474,11 +6486,11 @@
     <row r="74" spans="1:5">
       <c r="A74">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>66</v>
       </c>
       <c r="B74">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C74">
         <v>46</v>
@@ -6494,11 +6506,11 @@
     <row r="75" spans="1:5">
       <c r="A75">
         <f t="shared" ca="1" si="3"/>
-        <v>66</v>
+        <v>4</v>
       </c>
       <c r="B75">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75">
         <v>74</v>
@@ -6514,7 +6526,7 @@
     <row r="76" spans="1:5">
       <c r="A76">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B76">
         <f t="shared" ca="1" si="4"/>
@@ -6534,11 +6546,11 @@
     <row r="77" spans="1:5">
       <c r="A77">
         <f t="shared" ca="1" si="3"/>
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B77">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C77">
         <v>46</v>
@@ -6554,7 +6566,7 @@
     <row r="78" spans="1:5">
       <c r="A78">
         <f t="shared" ca="1" si="3"/>
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="B78">
         <f t="shared" ca="1" si="4"/>
@@ -6574,7 +6586,7 @@
     <row r="79" spans="1:5">
       <c r="A79">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="B79">
         <f t="shared" ca="1" si="4"/>
@@ -6594,7 +6606,7 @@
     <row r="80" spans="1:5">
       <c r="A80">
         <f t="shared" ca="1" si="3"/>
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B80">
         <f t="shared" ca="1" si="4"/>
@@ -6614,7 +6626,7 @@
     <row r="81" spans="1:5">
       <c r="A81">
         <f t="shared" ca="1" si="3"/>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B81">
         <f t="shared" ca="1" si="4"/>
@@ -6634,11 +6646,11 @@
     <row r="82" spans="1:5">
       <c r="A82">
         <f t="shared" ca="1" si="3"/>
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B82">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C82">
         <v>69</v>
@@ -6654,7 +6666,7 @@
     <row r="83" spans="1:5">
       <c r="A83">
         <f t="shared" ca="1" si="3"/>
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B83">
         <f t="shared" ca="1" si="4"/>
@@ -6674,11 +6686,11 @@
     <row r="84" spans="1:5">
       <c r="A84">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B84">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C84">
         <v>45</v>
@@ -6694,11 +6706,11 @@
     <row r="85" spans="1:5">
       <c r="A85">
         <f t="shared" ca="1" si="3"/>
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B85">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C85">
         <v>3</v>
@@ -6714,11 +6726,11 @@
     <row r="86" spans="1:5">
       <c r="A86">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B86">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86">
         <v>39</v>
@@ -6734,11 +6746,11 @@
     <row r="87" spans="1:5">
       <c r="A87">
         <f t="shared" ca="1" si="3"/>
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="B87">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87">
         <v>33</v>
@@ -6754,7 +6766,7 @@
     <row r="88" spans="1:5">
       <c r="A88">
         <f t="shared" ca="1" si="3"/>
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B88">
         <f t="shared" ca="1" si="4"/>
@@ -6774,7 +6786,7 @@
     <row r="89" spans="1:5">
       <c r="A89">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B89">
         <f t="shared" ca="1" si="4"/>
@@ -6794,11 +6806,11 @@
     <row r="90" spans="1:5">
       <c r="A90">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B90">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C90">
         <v>98</v>
@@ -6814,11 +6826,11 @@
     <row r="91" spans="1:5">
       <c r="A91">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="B91">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C91">
         <v>16</v>
@@ -6834,7 +6846,7 @@
     <row r="92" spans="1:5">
       <c r="A92">
         <f t="shared" ca="1" si="3"/>
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B92">
         <f t="shared" ca="1" si="4"/>
@@ -6854,7 +6866,7 @@
     <row r="93" spans="1:5">
       <c r="A93">
         <f t="shared" ca="1" si="3"/>
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B93">
         <f t="shared" ca="1" si="4"/>
@@ -6874,7 +6886,7 @@
     <row r="94" spans="1:5">
       <c r="A94">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B94">
         <f t="shared" ca="1" si="4"/>
@@ -6894,11 +6906,11 @@
     <row r="95" spans="1:5">
       <c r="A95">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B95">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C95">
         <v>36</v>
@@ -6914,7 +6926,7 @@
     <row r="96" spans="1:5">
       <c r="A96">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B96">
         <f t="shared" ca="1" si="4"/>
@@ -6934,11 +6946,11 @@
     <row r="97" spans="1:5">
       <c r="A97">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="B97">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C97">
         <v>49</v>
@@ -6954,11 +6966,11 @@
     <row r="98" spans="1:5">
       <c r="A98">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B98">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C98">
         <v>94</v>
@@ -6974,11 +6986,11 @@
     <row r="99" spans="1:5">
       <c r="A99">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B99">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C99">
         <v>62</v>
@@ -6994,11 +7006,11 @@
     <row r="100" spans="1:5">
       <c r="A100">
         <f t="shared" ca="1" si="3"/>
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="B100">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C100">
         <v>32</v>
@@ -7014,11 +7026,11 @@
     <row r="101" spans="1:5">
       <c r="A101">
         <f t="shared" ca="1" si="3"/>
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B101">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C101">
         <v>73</v>
@@ -7034,11 +7046,11 @@
     <row r="102" spans="1:5">
       <c r="A102">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="B102">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C102">
         <v>87</v>
@@ -7054,11 +7066,11 @@
     <row r="103" spans="1:5">
       <c r="A103">
         <f t="shared" ca="1" si="3"/>
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="B103">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C103">
         <v>58</v>
@@ -7074,11 +7086,11 @@
     <row r="104" spans="1:5">
       <c r="A104">
         <f t="shared" ca="1" si="3"/>
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B104">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C104">
         <v>19</v>
@@ -7094,11 +7106,11 @@
     <row r="105" spans="1:5">
       <c r="A105">
         <f t="shared" ca="1" si="3"/>
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B105">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C105">
         <v>6</v>
@@ -7114,7 +7126,7 @@
     <row r="106" spans="1:5">
       <c r="A106">
         <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <v>94</v>
       </c>
       <c r="B106">
         <f t="shared" ca="1" si="4"/>
@@ -7134,11 +7146,11 @@
     <row r="107" spans="1:5">
       <c r="A107">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="B107">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C107">
         <v>53</v>
@@ -7154,11 +7166,11 @@
     <row r="108" spans="1:5">
       <c r="A108">
         <f t="shared" ca="1" si="3"/>
-        <v>99</v>
+        <v>9</v>
       </c>
       <c r="B108">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C108">
         <v>19</v>
@@ -7174,11 +7186,11 @@
     <row r="109" spans="1:5">
       <c r="A109">
         <f t="shared" ca="1" si="3"/>
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B109">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C109">
         <v>93</v>
@@ -7194,11 +7206,11 @@
     <row r="110" spans="1:5">
       <c r="A110">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B110">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C110">
         <v>35</v>
@@ -7214,11 +7226,11 @@
     <row r="111" spans="1:5">
       <c r="A111">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B111">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C111">
         <v>8</v>
@@ -7234,7 +7246,7 @@
     <row r="112" spans="1:5">
       <c r="A112">
         <f t="shared" ca="1" si="3"/>
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B112">
         <f t="shared" ca="1" si="4"/>
@@ -7254,11 +7266,11 @@
     <row r="113" spans="1:5">
       <c r="A113">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="B113">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C113">
         <v>25</v>
@@ -7274,11 +7286,11 @@
     <row r="114" spans="1:5">
       <c r="A114">
         <f t="shared" ca="1" si="3"/>
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="B114">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C114">
         <v>94</v>
@@ -7294,11 +7306,11 @@
     <row r="115" spans="1:5">
       <c r="A115">
         <f t="shared" ca="1" si="3"/>
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="B115">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C115">
         <v>22</v>
@@ -7314,11 +7326,11 @@
     <row r="116" spans="1:5">
       <c r="A116">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B116">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C116">
         <v>52</v>
@@ -7334,11 +7346,11 @@
     <row r="117" spans="1:5">
       <c r="A117">
         <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B117">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C117">
         <v>68</v>
@@ -7354,11 +7366,11 @@
     <row r="118" spans="1:5">
       <c r="A118">
         <f t="shared" ca="1" si="3"/>
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B118">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C118">
         <v>82</v>
@@ -7374,11 +7386,11 @@
     <row r="119" spans="1:5">
       <c r="A119">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B119">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C119">
         <v>57</v>
@@ -7394,11 +7406,11 @@
     <row r="120" spans="1:5">
       <c r="A120">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="B120">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C120">
         <v>75</v>
@@ -7414,11 +7426,11 @@
     <row r="121" spans="1:5">
       <c r="A121">
         <f t="shared" ca="1" si="3"/>
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="B121">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C121">
         <v>53</v>
@@ -7434,11 +7446,11 @@
     <row r="122" spans="1:5">
       <c r="A122">
         <f t="shared" ca="1" si="3"/>
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="B122">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C122">
         <v>11</v>
@@ -7454,7 +7466,7 @@
     <row r="123" spans="1:5">
       <c r="A123">
         <f t="shared" ca="1" si="3"/>
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="B123">
         <f t="shared" ca="1" si="4"/>
@@ -7474,11 +7486,11 @@
     <row r="124" spans="1:5">
       <c r="A124">
         <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="B124">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C124">
         <v>51</v>
@@ -7494,11 +7506,11 @@
     <row r="125" spans="1:5">
       <c r="A125">
         <f t="shared" ca="1" si="3"/>
-        <v>94</v>
+        <v>51</v>
       </c>
       <c r="B125">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C125">
         <v>78</v>
@@ -7514,11 +7526,11 @@
     <row r="126" spans="1:5">
       <c r="A126">
         <f t="shared" ca="1" si="3"/>
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="B126">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C126">
         <v>78</v>
@@ -7534,11 +7546,11 @@
     <row r="127" spans="1:5">
       <c r="A127">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B127">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C127">
         <v>38</v>
@@ -7554,7 +7566,7 @@
     <row r="128" spans="1:5">
       <c r="A128">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B128">
         <f t="shared" ca="1" si="4"/>
@@ -7574,11 +7586,11 @@
     <row r="129" spans="1:5">
       <c r="A129">
         <f t="shared" ca="1" si="3"/>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B129">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C129">
         <v>40</v>
@@ -7594,11 +7606,11 @@
     <row r="130" spans="1:5">
       <c r="A130">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="B130">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C130">
         <v>67</v>
@@ -7613,11 +7625,11 @@
     </row>
     <row r="131" spans="1:5">
       <c r="A131">
-        <f t="shared" ref="A131:C141" ca="1" si="6">CEILING(RAND()*99,1)</f>
-        <v>49</v>
+        <f t="shared" ref="A131:A141" ca="1" si="6">CEILING(RAND()*99,1)</f>
+        <v>75</v>
       </c>
       <c r="B131">
-        <f t="shared" ref="B131:D141" ca="1" si="7">CEILING(RAND()*3,1)</f>
+        <f t="shared" ref="B131:B141" ca="1" si="7">CEILING(RAND()*3,1)</f>
         <v>3</v>
       </c>
       <c r="C131">
@@ -7634,11 +7646,11 @@
     <row r="132" spans="1:5">
       <c r="A132">
         <f t="shared" ca="1" si="6"/>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B132">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C132">
         <v>15</v>
@@ -7654,11 +7666,11 @@
     <row r="133" spans="1:5">
       <c r="A133">
         <f t="shared" ca="1" si="6"/>
-        <v>84</v>
+        <v>11</v>
       </c>
       <c r="B133">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C133">
         <v>17</v>
@@ -7674,7 +7686,7 @@
     <row r="134" spans="1:5">
       <c r="A134">
         <f t="shared" ca="1" si="6"/>
-        <v>45</v>
+        <v>95</v>
       </c>
       <c r="B134">
         <f t="shared" ca="1" si="7"/>
@@ -7694,11 +7706,11 @@
     <row r="135" spans="1:5">
       <c r="A135">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="B135">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C135">
         <v>83</v>
@@ -7714,7 +7726,7 @@
     <row r="136" spans="1:5">
       <c r="A136">
         <f t="shared" ca="1" si="6"/>
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="B136">
         <f t="shared" ca="1" si="7"/>
@@ -7734,11 +7746,11 @@
     <row r="137" spans="1:5">
       <c r="A137">
         <f t="shared" ca="1" si="6"/>
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="B137">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C137">
         <v>85</v>
@@ -7754,11 +7766,11 @@
     <row r="138" spans="1:5">
       <c r="A138">
         <f t="shared" ca="1" si="6"/>
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B138">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C138">
         <v>66</v>
@@ -7774,11 +7786,11 @@
     <row r="139" spans="1:5">
       <c r="A139">
         <f t="shared" ca="1" si="6"/>
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="B139">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C139">
         <v>66</v>
@@ -7794,7 +7806,7 @@
     <row r="140" spans="1:5">
       <c r="A140">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B140">
         <f t="shared" ca="1" si="7"/>
@@ -7814,11 +7826,11 @@
     <row r="141" spans="1:5">
       <c r="A141">
         <f t="shared" ca="1" si="6"/>
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B141">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C141">
         <v>97</v>

</xml_diff>